<commit_message>
Updates Mapping_Meta, nvto, widoco
nvto, widoco
- ein paar richtige Beispiele (richtige Form)

mapping_meta
- mini fixes
</commit_message>
<xml_diff>
--- a/Mapping/Mapping_Metadatentabelle.xlsx
+++ b/Mapping/Mapping_Metadatentabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Dropbox\ITI\NVT_Data-Model\Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7A7C32-DA47-4400-A46D-2BB653279CBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0601C68B-0339-45D0-B5DC-2846990D11D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="927" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produktionen" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2619" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="627">
   <si>
     <t>Identifier / geeinigter Name</t>
   </si>
@@ -2669,8 +2669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4512,7 +4512,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F3" sqref="F3:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5497,8 +5497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7360,8 +7360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:XFD79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9017,10 +9017,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10310,6 +10310,28 @@
         <v>491</v>
       </c>
     </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="44" t="s">
+        <v>560</v>
+      </c>
+      <c r="B63" t="s">
+        <v>568</v>
+      </c>
+      <c r="D63" s="37"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="23" t="s">
+        <v>566</v>
+      </c>
+      <c r="G63" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="H63" s="24" t="s">
+        <v>566</v>
+      </c>
+      <c r="I63" s="27" t="s">
+        <v>567</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10317,10 +10339,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11414,6 +11436,28 @@
       </c>
       <c r="I52" s="32" t="s">
         <v>491</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="44" t="s">
+        <v>560</v>
+      </c>
+      <c r="B53" t="s">
+        <v>568</v>
+      </c>
+      <c r="D53" s="37"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="23" t="s">
+        <v>566</v>
+      </c>
+      <c r="G53" s="35" t="s">
+        <v>567</v>
+      </c>
+      <c r="H53" s="24" t="s">
+        <v>566</v>
+      </c>
+      <c r="I53" s="27" t="s">
+        <v>567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>